<commit_message>
refactored bottom tabs, finished upload.js and uploaded sample data
</commit_message>
<xml_diff>
--- a/utils/sample_data.xlsx
+++ b/utils/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangliyao/Documents/Liyao/NEU/CS5520/grocery-tracker/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2DF8EF-0766-934E-8111-109D56531DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431B5A21-AB26-FD4D-9C02-A3F0C2882BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="542">
   <si>
     <t>Name</t>
   </si>
@@ -16883,7 +16883,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L2"/>
+      <selection activeCell="A18" activeCellId="1" sqref="A10:K10 A18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19714,10 +19714,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254998BE-05DE-B940-B00C-D57AC5D31A53}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19786,6 +19786,58 @@
         <v>45374</v>
       </c>
     </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>3.99</v>
+      </c>
+      <c r="E3">
+        <v>3.4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>1.17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1">
+        <v>45368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>5.99</v>
+      </c>
+      <c r="E4">
+        <v>3.4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>1.76</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1">
+        <v>45359</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactored searchHeader and put it at Home header
</commit_message>
<xml_diff>
--- a/utils/sample_data.xlsx
+++ b/utils/sample_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangliyao/Documents/Liyao/NEU/CS5520/grocery-tracker/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431B5A21-AB26-FD4D-9C02-A3F0C2882BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE19C59-7ED1-614A-BE6F-2E0FE87B4E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPI 755934fdd14142128ea9e93eef7" sheetId="1" r:id="rId1"/>
@@ -16882,8 +16882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4135044B-0B08-864F-8243-541B08A1DBBD}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" activeCellId="1" sqref="A10:K10 A18:K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19716,7 +19716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254998BE-05DE-B940-B00C-D57AC5D31A53}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -19840,5 +19840,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reused Search screen for searching by categories
</commit_message>
<xml_diff>
--- a/utils/sample_data.xlsx
+++ b/utils/sample_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangliyao/Documents/Liyao/NEU/CS5520/grocery-tracker/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE19C59-7ED1-614A-BE6F-2E0FE87B4E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18308125-EFB7-2145-ABFB-429F90205106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="800" windowWidth="25800" windowHeight="17300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPI 755934fdd14142128ea9e93eef7" sheetId="1" r:id="rId1"/>
     <sheet name="produce" sheetId="2" r:id="rId2"/>
-    <sheet name="small" sheetId="3" r:id="rId3"/>
+    <sheet name="meat_small" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CPI 755934fdd14142128ea9e93eef7'!$A$1:$L$668</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="542">
   <si>
     <t>Name</t>
   </si>
@@ -1657,7 +1657,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1788,6 +1788,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2134,9 +2141,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2494,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L668"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A630" workbookViewId="0">
+      <selection activeCell="A668" sqref="A668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16882,7 +16891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4135044B-0B08-864F-8243-541B08A1DBBD}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -19713,133 +19722,246 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254998BE-05DE-B940-B00C-D57AC5D31A53}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247CE525-251B-AD4A-8DAE-2D234E7F43B5}">
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="E2">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
+        <v>35.01</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2">
-        <v>5.45</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1">
-        <v>45374</v>
-      </c>
+      <c r="G2" s="2">
+        <v>35.01</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="3">
+        <v>45366</v>
+      </c>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <v>3.99</v>
-      </c>
-      <c r="E3">
-        <v>3.4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3">
-        <v>1.17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="1">
-        <v>45368</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>24.23</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2">
+        <v>24.23</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3">
+        <v>45359</v>
+      </c>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>5.99</v>
-      </c>
-      <c r="E4">
-        <v>3.4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4">
-        <v>1.76</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="1">
-        <v>45359</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>28.64</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2">
+        <v>28.64</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="3">
+        <v>45326</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="3">
+        <v>45317</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>30.6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2">
+        <v>30.6</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="3">
+        <v>45277</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="3">
+        <v>45198</v>
+      </c>
+      <c r="L7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved UI for product related screens
</commit_message>
<xml_diff>
--- a/utils/sample_data.xlsx
+++ b/utils/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangliyao/Documents/Liyao/NEU/CS5520/grocery-tracker/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08306CEE-EE5E-EA44-A4E6-2F54993AE961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA6949A-CBAC-C446-9704-08550112366E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="800" windowWidth="25800" windowHeight="17300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="544">
   <si>
     <t>Name</t>
   </si>
@@ -1652,6 +1652,12 @@
   </si>
   <si>
     <t>珠江桥牌生抽王-500ml</t>
+  </si>
+  <si>
+    <t>https://images.costcobusinessdelivery.com/ImageDelivery/imageService?profileId=12027981&amp;itemId=203435&amp;recipeName=680</t>
+  </si>
+  <si>
+    <t>https://www.sbfoods-worldwide.com/products/search/h9f2g10000001a77-img/GoldenCurryMixHot220g(OnlyforCanada)_500_500_190.jpg</t>
   </si>
 </sst>
 </file>
@@ -2505,8 +2511,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L668"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:XFD76"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242:K242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2856,7 +2862,7 @@
         <v>45368</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3047,7 +3053,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>45359</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -3157,7 +3163,7 @@
         <v>45359</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -3186,7 +3192,7 @@
         <v>45357</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -3241,7 +3247,7 @@
         <v>45357</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -3281,7 +3287,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -3390,7 +3396,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3660,7 +3666,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -3786,7 +3792,7 @@
         <v>45350</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -3806,7 +3812,7 @@
         <v>45349</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -3826,7 +3832,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -3915,7 +3921,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -4148,7 +4154,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -4168,7 +4174,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>96</v>
       </c>
@@ -4254,7 +4260,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>99</v>
       </c>
@@ -4274,7 +4280,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>100</v>
       </c>
@@ -4314,7 +4320,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>102</v>
       </c>
@@ -4440,7 +4446,7 @@
         <v>45335</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>107</v>
       </c>
@@ -4460,7 +4466,7 @@
         <v>45335</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>108</v>
       </c>
@@ -4506,7 +4512,7 @@
         <v>45331</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -4546,7 +4552,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>58</v>
       </c>
@@ -4586,7 +4592,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>112</v>
       </c>
@@ -4606,7 +4612,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>113</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -4761,7 +4767,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>118</v>
       </c>
@@ -4801,7 +4807,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>120</v>
       </c>
@@ -4830,7 +4836,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>122</v>
       </c>
@@ -4928,7 +4934,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>125</v>
       </c>
@@ -5034,7 +5040,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>130</v>
       </c>
@@ -5074,7 +5080,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>132</v>
       </c>
@@ -5143,7 +5149,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>134</v>
       </c>
@@ -5163,7 +5169,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>135</v>
       </c>
@@ -5209,7 +5215,7 @@
         <v>45321</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>136</v>
       </c>
@@ -5229,7 +5235,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>137</v>
       </c>
@@ -5269,7 +5275,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>139</v>
       </c>
@@ -5289,7 +5295,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>35</v>
       </c>
@@ -5413,7 +5419,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>142</v>
       </c>
@@ -5433,7 +5439,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -5513,7 +5519,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -5568,7 +5574,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>148</v>
       </c>
@@ -5648,7 +5654,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -5754,7 +5760,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>156</v>
       </c>
@@ -5886,7 +5892,7 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>159</v>
       </c>
@@ -5972,7 +5978,7 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>162</v>
       </c>
@@ -6070,7 +6076,7 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>165</v>
       </c>
@@ -6130,7 +6136,7 @@
         <v>45307</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>167</v>
       </c>
@@ -6150,7 +6156,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>168</v>
       </c>
@@ -6256,7 +6262,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -6276,7 +6282,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>68</v>
       </c>
@@ -6296,7 +6302,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>172</v>
       </c>
@@ -6336,7 +6342,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>174</v>
       </c>
@@ -6396,7 +6402,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>177</v>
       </c>
@@ -6456,7 +6462,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>179</v>
       </c>
@@ -6476,7 +6482,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>180</v>
       </c>
@@ -6496,7 +6502,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>181</v>
       </c>
@@ -6628,7 +6634,7 @@
         <v>45298</v>
       </c>
     </row>
-    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>185</v>
       </c>
@@ -6648,7 +6654,7 @@
         <v>45298</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>186</v>
       </c>
@@ -6688,7 +6694,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>188</v>
       </c>
@@ -6708,7 +6714,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>189</v>
       </c>
@@ -6849,7 +6855,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -7004,7 +7010,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>197</v>
       </c>
@@ -7056,7 +7062,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>199</v>
       </c>
@@ -7096,7 +7102,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>201</v>
       </c>
@@ -7401,7 +7407,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>209</v>
       </c>
@@ -7421,7 +7427,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>210</v>
       </c>
@@ -7441,7 +7447,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>179</v>
       </c>
@@ -7501,7 +7507,7 @@
         <v>45281</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>212</v>
       </c>
@@ -7521,7 +7527,7 @@
         <v>45281</v>
       </c>
     </row>
-    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>146</v>
       </c>
@@ -7550,7 +7556,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>213</v>
       </c>
@@ -7619,7 +7625,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>216</v>
       </c>
@@ -7679,7 +7685,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>219</v>
       </c>
@@ -7699,7 +7705,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>220</v>
       </c>
@@ -7797,7 +7803,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>222</v>
       </c>
@@ -7817,7 +7823,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>223</v>
       </c>
@@ -7880,7 +7886,7 @@
         <v>45279</v>
       </c>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>226</v>
       </c>
@@ -7900,7 +7906,7 @@
         <v>45279</v>
       </c>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>227</v>
       </c>
@@ -7920,7 +7926,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>228</v>
       </c>
@@ -7940,7 +7946,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>229</v>
       </c>
@@ -7960,7 +7966,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>35</v>
       </c>
@@ -8135,7 +8141,7 @@
         <v>45273</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>235</v>
       </c>
@@ -8155,7 +8161,7 @@
         <v>45273</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>48</v>
       </c>
@@ -8178,7 +8184,7 @@
         <v>45273</v>
       </c>
     </row>
-    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>236</v>
       </c>
@@ -8218,7 +8224,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>99</v>
       </c>
@@ -8238,7 +8244,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>237</v>
       </c>
@@ -8416,7 +8422,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>245</v>
       </c>
@@ -8436,7 +8442,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>246</v>
       </c>
@@ -8631,7 +8637,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>254</v>
       </c>
@@ -8712,7 +8718,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>257</v>
       </c>
@@ -9030,7 +9036,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>267</v>
       </c>
@@ -9139,7 +9145,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>271</v>
       </c>
@@ -9159,7 +9165,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>272</v>
       </c>
@@ -9328,7 +9334,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>278</v>
       </c>
@@ -9348,7 +9354,7 @@
         <v>45251</v>
       </c>
     </row>
-    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>279</v>
       </c>
@@ -9414,7 +9420,7 @@
         <v>45251</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>281</v>
       </c>
@@ -9434,7 +9440,7 @@
         <v>45251</v>
       </c>
     </row>
-    <row r="311" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>282</v>
       </c>
@@ -9474,7 +9480,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>188</v>
       </c>
@@ -9554,7 +9560,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>284</v>
       </c>
@@ -9574,7 +9580,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>285</v>
       </c>
@@ -9614,7 +9620,7 @@
         <v>45246</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>130</v>
       </c>
@@ -9634,7 +9640,7 @@
         <v>45246</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>287</v>
       </c>
@@ -9654,7 +9660,7 @@
         <v>45246</v>
       </c>
     </row>
-    <row r="322" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>288</v>
       </c>
@@ -9674,7 +9680,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="323" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>289</v>
       </c>
@@ -9694,7 +9700,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="324" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>290</v>
       </c>
@@ -9734,7 +9740,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="326" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>292</v>
       </c>
@@ -9814,7 +9820,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="330" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>295</v>
       </c>
@@ -9874,7 +9880,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="333" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>100</v>
       </c>
@@ -9894,7 +9900,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="334" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>298</v>
       </c>
@@ -9914,7 +9920,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="335" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>299</v>
       </c>
@@ -9934,7 +9940,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="336" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>300</v>
       </c>
@@ -9994,7 +10000,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="339" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>303</v>
       </c>
@@ -10069,7 +10075,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>109</v>
       </c>
@@ -10089,7 +10095,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>287</v>
       </c>
@@ -10295,7 +10301,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="353" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>309</v>
       </c>
@@ -10315,7 +10321,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="354" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>310</v>
       </c>
@@ -10375,7 +10381,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="357" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>312</v>
       </c>
@@ -10404,7 +10410,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="358" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>314</v>
       </c>
@@ -10424,7 +10430,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="359" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>315</v>
       </c>
@@ -10444,7 +10450,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="360" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>316</v>
       </c>
@@ -10544,7 +10550,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>321</v>
       </c>
@@ -10564,7 +10570,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>322</v>
       </c>
@@ -10584,7 +10590,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="367" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>323</v>
       </c>
@@ -10604,7 +10610,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="368" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>324</v>
       </c>
@@ -10696,7 +10702,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="372" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>326</v>
       </c>
@@ -10716,7 +10722,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="373" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>327</v>
       </c>
@@ -10736,7 +10742,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="374" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>228</v>
       </c>
@@ -10756,7 +10762,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="375" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>58</v>
       </c>
@@ -10845,7 +10851,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="379" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>330</v>
       </c>
@@ -10963,7 +10969,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="384" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>333</v>
       </c>
@@ -10983,7 +10989,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="385" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>334</v>
       </c>
@@ -11023,7 +11029,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="387" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>336</v>
       </c>
@@ -11043,7 +11049,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>337</v>
       </c>
@@ -11123,7 +11129,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>340</v>
       </c>
@@ -11163,7 +11169,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>342</v>
       </c>
@@ -11183,7 +11189,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>343</v>
       </c>
@@ -11203,7 +11209,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>292</v>
       </c>
@@ -11269,7 +11275,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>345</v>
       </c>
@@ -11418,7 +11424,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>350</v>
       </c>
@@ -11458,7 +11464,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>351</v>
       </c>
@@ -11498,7 +11504,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="410" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>353</v>
       </c>
@@ -11518,7 +11524,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>354</v>
       </c>
@@ -11578,7 +11584,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>167</v>
       </c>
@@ -11598,7 +11604,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="415" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>357</v>
       </c>
@@ -11618,7 +11624,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>358</v>
       </c>
@@ -11638,7 +11644,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="417" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>359</v>
       </c>
@@ -11658,7 +11664,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="418" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>360</v>
       </c>
@@ -11678,7 +11684,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>361</v>
       </c>
@@ -11827,7 +11833,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>364</v>
       </c>
@@ -11887,7 +11893,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>235</v>
       </c>
@@ -11907,7 +11913,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="430" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>367</v>
       </c>
@@ -12067,7 +12073,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="438" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>374</v>
       </c>
@@ -12136,7 +12142,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="441" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>376</v>
       </c>
@@ -12156,7 +12162,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="442" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>377</v>
       </c>
@@ -12176,7 +12182,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="443" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>378</v>
       </c>
@@ -12322,7 +12328,7 @@
         <v>45206</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>381</v>
       </c>
@@ -12402,7 +12408,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="454" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>210</v>
       </c>
@@ -12422,7 +12428,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="455" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>385</v>
       </c>
@@ -12442,7 +12448,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="456" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>386</v>
       </c>
@@ -12502,7 +12508,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="459" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>389</v>
       </c>
@@ -12637,7 +12643,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="465" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>391</v>
       </c>
@@ -12657,7 +12663,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="466" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>392</v>
       </c>
@@ -12797,7 +12803,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="473" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>397</v>
       </c>
@@ -12969,7 +12975,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="481" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>405</v>
       </c>
@@ -13038,7 +13044,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="484" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>408</v>
       </c>
@@ -13164,7 +13170,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="490" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>412</v>
       </c>
@@ -13184,7 +13190,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="491" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>413</v>
       </c>
@@ -13204,7 +13210,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="492" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>414</v>
       </c>
@@ -13224,7 +13230,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="493" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>415</v>
       </c>
@@ -13244,7 +13250,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="494" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>416</v>
       </c>
@@ -13264,7 +13270,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="495" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>361</v>
       </c>
@@ -13284,7 +13290,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="496" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>417</v>
       </c>
@@ -13544,7 +13550,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="509" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
         <v>428</v>
       </c>
@@ -13584,7 +13590,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="511" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
         <v>430</v>
       </c>
@@ -13676,7 +13682,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="515" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>109</v>
       </c>
@@ -13911,7 +13917,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="526" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
         <v>438</v>
       </c>
@@ -13971,7 +13977,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="529" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>441</v>
       </c>
@@ -14000,7 +14006,7 @@
         <v>45182</v>
       </c>
     </row>
-    <row r="530" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>442</v>
       </c>
@@ -14020,7 +14026,7 @@
         <v>45182</v>
       </c>
     </row>
-    <row r="531" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>443</v>
       </c>
@@ -14040,7 +14046,7 @@
         <v>45182</v>
       </c>
     </row>
-    <row r="532" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>444</v>
       </c>
@@ -14060,7 +14066,7 @@
         <v>45182</v>
       </c>
     </row>
-    <row r="533" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>445</v>
       </c>
@@ -14080,7 +14086,7 @@
         <v>45182</v>
       </c>
     </row>
-    <row r="534" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>446</v>
       </c>
@@ -14100,7 +14106,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="535" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>447</v>
       </c>
@@ -14120,7 +14126,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="536" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>448</v>
       </c>
@@ -14200,7 +14206,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="540" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>450</v>
       </c>
@@ -14260,7 +14266,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="543" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>452</v>
       </c>
@@ -14466,7 +14472,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="553" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
         <v>460</v>
       </c>
@@ -14486,7 +14492,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="554" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>461</v>
       </c>
@@ -14546,7 +14552,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="557" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
         <v>463</v>
       </c>
@@ -14566,7 +14572,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="558" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
         <v>464</v>
       </c>
@@ -14586,7 +14592,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="559" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
         <v>201</v>
       </c>
@@ -14606,7 +14612,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="560" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
         <v>139</v>
       </c>
@@ -14626,7 +14632,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="561" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>465</v>
       </c>
@@ -14812,7 +14818,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="570" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
         <v>470</v>
       </c>
@@ -14898,7 +14904,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="574" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
         <v>472</v>
       </c>
@@ -14918,7 +14924,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="575" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
         <v>473</v>
       </c>
@@ -14967,7 +14973,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="577" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
         <v>475</v>
       </c>
@@ -15007,7 +15013,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="579" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
         <v>477</v>
       </c>
@@ -15027,7 +15033,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="580" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
         <v>478</v>
       </c>
@@ -15127,7 +15133,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="585" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
         <v>361</v>
       </c>
@@ -15147,7 +15153,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="586" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="586" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
         <v>482</v>
       </c>
@@ -15213,7 +15219,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="589" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
         <v>484</v>
       </c>
@@ -15253,7 +15259,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="591" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
         <v>485</v>
       </c>
@@ -15273,7 +15279,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="592" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
         <v>486</v>
       </c>
@@ -15293,7 +15299,7 @@
         <v>45168</v>
       </c>
     </row>
-    <row r="593" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
         <v>191</v>
       </c>
@@ -15333,7 +15339,7 @@
         <v>45168</v>
       </c>
     </row>
-    <row r="595" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
         <v>488</v>
       </c>
@@ -15353,7 +15359,7 @@
         <v>45168</v>
       </c>
     </row>
-    <row r="596" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
         <v>489</v>
       </c>
@@ -15419,7 +15425,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="599" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
         <v>490</v>
       </c>
@@ -15548,7 +15554,7 @@
         <v>45164</v>
       </c>
     </row>
-    <row r="605" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
         <v>493</v>
       </c>
@@ -15568,7 +15574,7 @@
         <v>45164</v>
       </c>
     </row>
-    <row r="606" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
         <v>494</v>
       </c>
@@ -15588,7 +15594,7 @@
         <v>45164</v>
       </c>
     </row>
-    <row r="607" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
         <v>495</v>
       </c>
@@ -15608,7 +15614,7 @@
         <v>45164</v>
       </c>
     </row>
-    <row r="608" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
         <v>496</v>
       </c>
@@ -15628,7 +15634,7 @@
         <v>45164</v>
       </c>
     </row>
-    <row r="609" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
         <v>498</v>
       </c>
@@ -15763,7 +15769,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="615" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A615" t="s">
         <v>470</v>
       </c>
@@ -15803,7 +15809,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="617" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A617" t="s">
         <v>189</v>
       </c>
@@ -15969,7 +15975,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="625" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
         <v>510</v>
       </c>
@@ -15989,7 +15995,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="626" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
         <v>511</v>
       </c>
@@ -16029,7 +16035,7 @@
         <v>45155</v>
       </c>
     </row>
-    <row r="628" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A628" t="s">
         <v>513</v>
       </c>
@@ -16149,7 +16155,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="634" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="634" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A634" t="s">
         <v>516</v>
       </c>
@@ -16189,7 +16195,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="636" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A636" t="s">
         <v>518</v>
       </c>
@@ -16407,7 +16413,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="646" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="646" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A646" t="s">
         <v>523</v>
       </c>
@@ -16427,7 +16433,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="647" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="647" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A647" t="s">
         <v>524</v>
       </c>
@@ -16447,7 +16453,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="648" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="648" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A648" t="s">
         <v>525</v>
       </c>
@@ -16467,7 +16473,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="649" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="649" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A649" t="s">
         <v>526</v>
       </c>
@@ -16487,7 +16493,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="650" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="650" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A650" t="s">
         <v>527</v>
       </c>
@@ -16527,7 +16533,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="652" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="652" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A652" t="s">
         <v>529</v>
       </c>
@@ -16567,7 +16573,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="654" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="654" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A654" t="s">
         <v>531</v>
       </c>
@@ -16656,7 +16662,7 @@
         <v>45150</v>
       </c>
     </row>
-    <row r="658" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="658" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
         <v>533</v>
       </c>
@@ -16676,7 +16682,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="659" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
         <v>534</v>
       </c>
@@ -16696,7 +16702,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="660" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="660" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
         <v>535</v>
       </c>
@@ -16716,7 +16722,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="661" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
         <v>536</v>
       </c>
@@ -16776,7 +16782,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="664" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="664" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
         <v>539</v>
       </c>
@@ -16796,7 +16802,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="665" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
         <v>540</v>
       </c>
@@ -16845,7 +16851,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="667" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="667" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
         <v>541</v>
       </c>
@@ -16889,7 +16895,7 @@
   <autoFilter ref="A1:L668" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="8">
       <filters>
-        <filter val="Meat"/>
+        <filter val="Groceries"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -16903,7 +16909,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19980,10 +19986,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14458C0-5F51-434B-B68D-A2BAF9BBF511}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20028,25 +20034,61 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
       </c>
       <c r="D2">
-        <v>37.21</v>
+        <v>18.989999999999998</v>
+      </c>
+      <c r="E2">
+        <v>1.36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>13.96</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="K2" s="1">
-        <v>45336</v>
+        <v>45315</v>
+      </c>
+      <c r="L2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3">
+        <v>3.48</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="1">
+        <v>45277</v>
+      </c>
+      <c r="L3" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved UI & fixed deletion bug
</commit_message>
<xml_diff>
--- a/utils/sample_data.xlsx
+++ b/utils/sample_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangliyao/Documents/Liyao/NEU/CS5520/grocery-tracker/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA6949A-CBAC-C446-9704-08550112366E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4299C4-B733-A445-895E-D87843C039BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="800" windowWidth="25800" windowHeight="17300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="800" windowWidth="25800" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPI 755934fdd14142128ea9e93eef7" sheetId="1" r:id="rId1"/>
@@ -2508,10 +2508,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L668"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A242" sqref="A242:K242"/>
     </sheetView>
   </sheetViews>
@@ -2558,7 +2557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>45374</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2616,7 +2615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>45374</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>45374</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>45374</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>45373</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2752,7 +2751,7 @@
         <v>45373</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2781,7 +2780,7 @@
         <v>45373</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2807,7 +2806,7 @@
         <v>45368</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>45368</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>45368</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2891,7 +2890,7 @@
         <v>45366</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>45366</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -2946,7 +2945,7 @@
         <v>45366</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>45366</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -3001,7 +3000,7 @@
         <v>45366</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3053,7 +3052,7 @@
         <v>45363</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>45359</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -3111,7 +3110,7 @@
         <v>45359</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>45359</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>45357</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -3267,7 +3266,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -3327,7 +3326,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -3347,7 +3346,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -3376,7 +3375,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -3416,7 +3415,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3465,7 +3464,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -3491,7 +3490,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -3517,7 +3516,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -3537,7 +3536,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -3557,7 +3556,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -3577,7 +3576,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -3597,7 +3596,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3626,7 +3625,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -3646,7 +3645,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -3666,7 +3665,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -3686,7 +3685,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -3706,7 +3705,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -3732,7 +3731,7 @@
         <v>45351</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -3752,7 +3751,7 @@
         <v>45351</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -3772,7 +3771,7 @@
         <v>45351</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>84</v>
       </c>
@@ -3792,7 +3791,7 @@
         <v>45350</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -3832,7 +3831,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -3881,7 +3880,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -3901,7 +3900,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -3941,7 +3940,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>45</v>
       </c>
@@ -3967,7 +3966,7 @@
         <v>45347</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>91</v>
       </c>
@@ -3987,7 +3986,7 @@
         <v>45345</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -4013,7 +4012,7 @@
         <v>45345</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>29</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>45345</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>92</v>
       </c>
@@ -4059,7 +4058,7 @@
         <v>45340</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -4079,7 +4078,7 @@
         <v>45340</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>32</v>
       </c>
@@ -4105,7 +4104,7 @@
         <v>45338</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>93</v>
       </c>
@@ -4134,7 +4133,7 @@
         <v>45338</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>94</v>
       </c>
@@ -4154,7 +4153,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -4194,7 +4193,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -4220,7 +4219,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>97</v>
       </c>
@@ -4240,7 +4239,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>98</v>
       </c>
@@ -4300,7 +4299,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>101</v>
       </c>
@@ -4320,7 +4319,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>102</v>
       </c>
@@ -4340,7 +4339,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>103</v>
       </c>
@@ -4360,7 +4359,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>104</v>
       </c>
@@ -4380,7 +4379,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>105</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>45336</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>106</v>
       </c>
@@ -4420,7 +4419,7 @@
         <v>45335</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -4446,7 +4445,7 @@
         <v>45335</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>107</v>
       </c>
@@ -4486,7 +4485,7 @@
         <v>45331</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -4512,7 +4511,7 @@
         <v>45331</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -4532,7 +4531,7 @@
         <v>45331</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>110</v>
       </c>
@@ -4572,7 +4571,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>111</v>
       </c>
@@ -4632,7 +4631,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -4652,7 +4651,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>39</v>
       </c>
@@ -4678,7 +4677,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>40</v>
       </c>
@@ -4707,7 +4706,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>103</v>
       </c>
@@ -4727,7 +4726,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>115</v>
       </c>
@@ -4747,7 +4746,7 @@
         <v>45329</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>116</v>
       </c>
@@ -4787,7 +4786,7 @@
         <v>45328</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>119</v>
       </c>
@@ -4807,7 +4806,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>120</v>
       </c>
@@ -4856,7 +4855,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>123</v>
       </c>
@@ -4876,7 +4875,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>75</v>
       </c>
@@ -4905,7 +4904,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>63</v>
       </c>
@@ -4954,7 +4953,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>126</v>
       </c>
@@ -4974,7 +4973,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>127</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>128</v>
       </c>
@@ -5014,7 +5013,7 @@
         <v>45326</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>129</v>
       </c>
@@ -5040,7 +5039,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>130</v>
       </c>
@@ -5060,7 +5059,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>131</v>
       </c>
@@ -5100,7 +5099,7 @@
         <v>45324</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>63</v>
       </c>
@@ -5129,7 +5128,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>133</v>
       </c>
@@ -5189,7 +5188,7 @@
         <v>45321</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>29</v>
       </c>
@@ -5255,7 +5254,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>138</v>
       </c>
@@ -5295,7 +5294,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>35</v>
       </c>
@@ -5324,7 +5323,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>140</v>
       </c>
@@ -5344,7 +5343,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>42</v>
       </c>
@@ -5370,7 +5369,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>63</v>
       </c>
@@ -5399,7 +5398,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -5459,7 +5458,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>97</v>
       </c>
@@ -5479,7 +5478,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -5499,7 +5498,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -5548,7 +5547,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -5594,7 +5593,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -5614,7 +5613,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>150</v>
       </c>
@@ -5634,7 +5633,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>92</v>
       </c>
@@ -5674,7 +5673,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -5700,7 +5699,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -5720,7 +5719,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>154</v>
       </c>
@@ -5740,7 +5739,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>155</v>
       </c>
@@ -5780,7 +5779,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>81</v>
       </c>
@@ -5800,7 +5799,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>157</v>
       </c>
@@ -5820,7 +5819,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>158</v>
       </c>
@@ -5846,7 +5845,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>126</v>
       </c>
@@ -5866,7 +5865,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>32</v>
       </c>
@@ -5912,7 +5911,7 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>23</v>
       </c>
@@ -5938,7 +5937,7 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>160</v>
       </c>
@@ -5958,7 +5957,7 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>161</v>
       </c>
@@ -5998,7 +5997,7 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>104</v>
       </c>
@@ -6018,7 +6017,7 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>63</v>
       </c>
@@ -6047,7 +6046,7 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>163</v>
       </c>
@@ -6096,7 +6095,7 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>166</v>
       </c>
@@ -6116,7 +6115,7 @@
         <v>45307</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>150</v>
       </c>
@@ -6176,7 +6175,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>104</v>
       </c>
@@ -6196,7 +6195,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -6222,7 +6221,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>169</v>
       </c>
@@ -6242,7 +6241,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>170</v>
       </c>
@@ -6322,7 +6321,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>173</v>
       </c>
@@ -6362,7 +6361,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>175</v>
       </c>
@@ -6382,7 +6381,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>176</v>
       </c>
@@ -6402,7 +6401,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>177</v>
       </c>
@@ -6422,7 +6421,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>126</v>
       </c>
@@ -6442,7 +6441,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>178</v>
       </c>
@@ -6462,7 +6461,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>179</v>
       </c>
@@ -6482,7 +6481,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>180</v>
       </c>
@@ -6522,7 +6521,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>182</v>
       </c>
@@ -6542,7 +6541,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>183</v>
       </c>
@@ -6568,7 +6567,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>32</v>
       </c>
@@ -6594,7 +6593,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>184</v>
       </c>
@@ -6614,7 +6613,7 @@
         <v>45303</v>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>157</v>
       </c>
@@ -6674,7 +6673,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>187</v>
       </c>
@@ -6694,7 +6693,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>188</v>
       </c>
@@ -6714,7 +6713,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>189</v>
       </c>
@@ -6734,7 +6733,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>61</v>
       </c>
@@ -6754,7 +6753,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>39</v>
       </c>
@@ -6780,7 +6779,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>89</v>
       </c>
@@ -6800,7 +6799,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>45</v>
       </c>
@@ -6826,7 +6825,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>190</v>
       </c>
@@ -6875,7 +6874,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>42</v>
       </c>
@@ -6901,7 +6900,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>192</v>
       </c>
@@ -6921,7 +6920,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>193</v>
       </c>
@@ -6941,7 +6940,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>194</v>
       </c>
@@ -6961,7 +6960,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>195</v>
       </c>
@@ -6981,7 +6980,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>196</v>
       </c>
@@ -7030,7 +7029,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>33</v>
       </c>
@@ -7082,7 +7081,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>200</v>
       </c>
@@ -7122,7 +7121,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>202</v>
       </c>
@@ -7142,7 +7141,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>140</v>
       </c>
@@ -7162,7 +7161,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>203</v>
       </c>
@@ -7182,7 +7181,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>204</v>
       </c>
@@ -7202,7 +7201,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>205</v>
       </c>
@@ -7222,7 +7221,7 @@
         <v>45289</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>206</v>
       </c>
@@ -7242,7 +7241,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>23</v>
       </c>
@@ -7271,7 +7270,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>29</v>
       </c>
@@ -7300,7 +7299,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>207</v>
       </c>
@@ -7326,7 +7325,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>131</v>
       </c>
@@ -7346,7 +7345,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>190</v>
       </c>
@@ -7378,7 +7377,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>33</v>
       </c>
@@ -7407,7 +7406,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>209</v>
       </c>
@@ -7447,7 +7446,7 @@
         <v>45284</v>
       </c>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>179</v>
       </c>
@@ -7467,7 +7466,7 @@
         <v>45281</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>69</v>
       </c>
@@ -7487,7 +7486,7 @@
         <v>45281</v>
       </c>
     </row>
-    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>211</v>
       </c>
@@ -7507,7 +7506,7 @@
         <v>45281</v>
       </c>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>212</v>
       </c>
@@ -7576,7 +7575,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>214</v>
       </c>
@@ -7605,7 +7604,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>215</v>
       </c>
@@ -7625,7 +7624,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>216</v>
       </c>
@@ -7645,7 +7644,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>217</v>
       </c>
@@ -7665,7 +7664,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>218</v>
       </c>
@@ -7725,7 +7724,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>221</v>
       </c>
@@ -7751,7 +7750,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>147</v>
       </c>
@@ -7777,7 +7776,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>152</v>
       </c>
@@ -7846,7 +7845,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>224</v>
       </c>
@@ -7866,7 +7865,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>225</v>
       </c>
@@ -7966,7 +7965,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>35</v>
       </c>
@@ -7995,7 +7994,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>230</v>
       </c>
@@ -8015,7 +8014,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>231</v>
       </c>
@@ -8035,7 +8034,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>232</v>
       </c>
@@ -8055,7 +8054,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>233</v>
       </c>
@@ -8075,7 +8074,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>234</v>
       </c>
@@ -8095,7 +8094,7 @@
         <v>45277</v>
       </c>
     </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>116</v>
       </c>
@@ -8115,7 +8114,7 @@
         <v>45273</v>
       </c>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>129</v>
       </c>
@@ -8141,7 +8140,7 @@
         <v>45273</v>
       </c>
     </row>
-    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>235</v>
       </c>
@@ -8161,7 +8160,7 @@
         <v>45273</v>
       </c>
     </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>48</v>
       </c>
@@ -8204,7 +8203,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>153</v>
       </c>
@@ -8244,7 +8243,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>237</v>
       </c>
@@ -8264,7 +8263,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>238</v>
       </c>
@@ -8284,7 +8283,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>239</v>
       </c>
@@ -8310,7 +8309,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>242</v>
       </c>
@@ -8330,7 +8329,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>158</v>
       </c>
@@ -8356,7 +8355,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>32</v>
       </c>
@@ -8382,7 +8381,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>243</v>
       </c>
@@ -8402,7 +8401,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>244</v>
       </c>
@@ -8442,7 +8441,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>246</v>
       </c>
@@ -8462,7 +8461,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>247</v>
       </c>
@@ -8482,7 +8481,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>248</v>
       </c>
@@ -8502,7 +8501,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>75</v>
       </c>
@@ -8531,7 +8530,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>249</v>
       </c>
@@ -8551,7 +8550,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>250</v>
       </c>
@@ -8571,7 +8570,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>251</v>
       </c>
@@ -8597,7 +8596,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>252</v>
       </c>
@@ -8617,7 +8616,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>253</v>
       </c>
@@ -8657,7 +8656,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>255</v>
       </c>
@@ -8686,7 +8685,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>26</v>
       </c>
@@ -8738,7 +8737,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>258</v>
       </c>
@@ -8758,7 +8757,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>89</v>
       </c>
@@ -8778,7 +8777,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>259</v>
       </c>
@@ -8798,7 +8797,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>260</v>
       </c>
@@ -8818,7 +8817,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>261</v>
       </c>
@@ -8838,7 +8837,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>262</v>
       </c>
@@ -8858,7 +8857,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>263</v>
       </c>
@@ -8878,7 +8877,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>264</v>
       </c>
@@ -8898,7 +8897,7 @@
         <v>45260</v>
       </c>
     </row>
-    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>45</v>
       </c>
@@ -8924,7 +8923,7 @@
         <v>45260</v>
       </c>
     </row>
-    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>20</v>
       </c>
@@ -8950,7 +8949,7 @@
         <v>45260</v>
       </c>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>23</v>
       </c>
@@ -8976,7 +8975,7 @@
         <v>45258</v>
       </c>
     </row>
-    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>265</v>
       </c>
@@ -8996,7 +8995,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>231</v>
       </c>
@@ -9016,7 +9015,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>266</v>
       </c>
@@ -9036,7 +9035,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>267</v>
       </c>
@@ -9056,7 +9055,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>268</v>
       </c>
@@ -9076,7 +9075,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>269</v>
       </c>
@@ -9096,7 +9095,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>270</v>
       </c>
@@ -9116,7 +9115,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>33</v>
       </c>
@@ -9165,7 +9164,7 @@
         <v>45257</v>
       </c>
     </row>
-    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>272</v>
       </c>
@@ -9185,7 +9184,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>89</v>
       </c>
@@ -9205,7 +9204,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>259</v>
       </c>
@@ -9225,7 +9224,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>273</v>
       </c>
@@ -9245,7 +9244,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>274</v>
       </c>
@@ -9265,7 +9264,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>275</v>
       </c>
@@ -9285,7 +9284,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>276</v>
       </c>
@@ -9305,7 +9304,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>277</v>
       </c>
@@ -9374,7 +9373,7 @@
         <v>45251</v>
       </c>
     </row>
-    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>45</v>
       </c>
@@ -9400,7 +9399,7 @@
         <v>45251</v>
       </c>
     </row>
-    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>280</v>
       </c>
@@ -9420,7 +9419,7 @@
         <v>45251</v>
       </c>
     </row>
-    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>281</v>
       </c>
@@ -9460,7 +9459,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>283</v>
       </c>
@@ -9480,7 +9479,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>188</v>
       </c>
@@ -9500,7 +9499,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="314" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>61</v>
       </c>
@@ -9520,7 +9519,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="315" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>231</v>
       </c>
@@ -9540,7 +9539,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>273</v>
       </c>
@@ -9600,7 +9599,7 @@
         <v>45247</v>
       </c>
     </row>
-    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>286</v>
       </c>
@@ -9620,7 +9619,7 @@
         <v>45246</v>
       </c>
     </row>
-    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>130</v>
       </c>
@@ -9640,7 +9639,7 @@
         <v>45246</v>
       </c>
     </row>
-    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>287</v>
       </c>
@@ -9720,7 +9719,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="325" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>291</v>
       </c>
@@ -9760,7 +9759,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="327" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>293</v>
       </c>
@@ -9780,7 +9779,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="328" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>294</v>
       </c>
@@ -9800,7 +9799,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="329" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>84</v>
       </c>
@@ -9840,7 +9839,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="331" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>296</v>
       </c>
@@ -9860,7 +9859,7 @@
         <v>45244</v>
       </c>
     </row>
-    <row r="332" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>297</v>
       </c>
@@ -9960,7 +9959,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>301</v>
       </c>
@@ -9980,7 +9979,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="338" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>302</v>
       </c>
@@ -10020,7 +10019,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="340" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>304</v>
       </c>
@@ -10049,7 +10048,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>23</v>
       </c>
@@ -10075,7 +10074,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="342" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>109</v>
       </c>
@@ -10095,7 +10094,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>287</v>
       </c>
@@ -10115,7 +10114,7 @@
         <v>45237</v>
       </c>
     </row>
-    <row r="344" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>306</v>
       </c>
@@ -10135,7 +10134,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="345" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>161</v>
       </c>
@@ -10155,7 +10154,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>307</v>
       </c>
@@ -10175,7 +10174,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="347" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>308</v>
       </c>
@@ -10195,7 +10194,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="348" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>242</v>
       </c>
@@ -10215,7 +10214,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="349" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>61</v>
       </c>
@@ -10235,7 +10234,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="350" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>231</v>
       </c>
@@ -10255,7 +10254,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>205</v>
       </c>
@@ -10275,7 +10274,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>39</v>
       </c>
@@ -10341,7 +10340,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="355" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>149</v>
       </c>
@@ -10361,7 +10360,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="356" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>311</v>
       </c>
@@ -10470,7 +10469,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="361" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>317</v>
       </c>
@@ -10490,7 +10489,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="362" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>318</v>
       </c>
@@ -10510,7 +10509,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="363" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>319</v>
       </c>
@@ -10530,7 +10529,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="364" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>320</v>
       </c>
@@ -10550,7 +10549,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="365" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>321</v>
       </c>
@@ -10570,7 +10569,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="366" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>322</v>
       </c>
@@ -10630,7 +10629,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="369" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>325</v>
       </c>
@@ -10650,7 +10649,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="370" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>147</v>
       </c>
@@ -10676,7 +10675,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="371" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>22</v>
       </c>
@@ -10782,7 +10781,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="376" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>328</v>
       </c>
@@ -10802,7 +10801,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="377" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>63</v>
       </c>
@@ -10831,7 +10830,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="378" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>329</v>
       </c>
@@ -10871,7 +10870,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="380" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>93</v>
       </c>
@@ -10900,7 +10899,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="381" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>331</v>
       </c>
@@ -10929,7 +10928,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="382" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>332</v>
       </c>
@@ -10949,7 +10948,7 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="383" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>82</v>
       </c>
@@ -11009,7 +11008,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="386" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>335</v>
       </c>
@@ -11049,7 +11048,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>337</v>
       </c>
@@ -11069,7 +11068,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>89</v>
       </c>
@@ -11089,7 +11088,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="390" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>338</v>
       </c>
@@ -11109,7 +11108,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="391" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>339</v>
       </c>
@@ -11129,7 +11128,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>340</v>
       </c>
@@ -11149,7 +11148,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="393" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>341</v>
       </c>
@@ -11229,7 +11228,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="397" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>344</v>
       </c>
@@ -11249,7 +11248,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>45</v>
       </c>
@@ -11275,7 +11274,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>345</v>
       </c>
@@ -11295,7 +11294,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="400" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>346</v>
       </c>
@@ -11315,7 +11314,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="401" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>347</v>
       </c>
@@ -11335,7 +11334,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="402" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>150</v>
       </c>
@@ -11355,7 +11354,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>184</v>
       </c>
@@ -11375,7 +11374,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="404" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>348</v>
       </c>
@@ -11395,7 +11394,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>349</v>
       </c>
@@ -11424,7 +11423,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="406" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>350</v>
       </c>
@@ -11444,7 +11443,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="407" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>280</v>
       </c>
@@ -11484,7 +11483,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="409" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>352</v>
       </c>
@@ -11544,7 +11543,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>355</v>
       </c>
@@ -11564,7 +11563,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="413" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>356</v>
       </c>
@@ -11684,7 +11683,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="419" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>361</v>
       </c>
@@ -11704,7 +11703,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="420" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>308</v>
       </c>
@@ -11724,7 +11723,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="421" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>362</v>
       </c>
@@ -11744,7 +11743,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="422" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>248</v>
       </c>
@@ -11764,7 +11763,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="423" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>75</v>
       </c>
@@ -11793,7 +11792,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="424" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>88</v>
       </c>
@@ -11813,7 +11812,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="425" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>363</v>
       </c>
@@ -11833,7 +11832,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="426" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>364</v>
       </c>
@@ -11853,7 +11852,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="427" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>365</v>
       </c>
@@ -11873,7 +11872,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="428" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>366</v>
       </c>
@@ -11893,7 +11892,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="429" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>235</v>
       </c>
@@ -11933,7 +11932,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="431" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>368</v>
       </c>
@@ -11953,7 +11952,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="432" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>369</v>
       </c>
@@ -11973,7 +11972,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="433" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>370</v>
       </c>
@@ -11993,7 +11992,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="434" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>371</v>
       </c>
@@ -12013,7 +12012,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="435" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>259</v>
       </c>
@@ -12033,7 +12032,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="436" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>372</v>
       </c>
@@ -12053,7 +12052,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="437" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>373</v>
       </c>
@@ -12093,7 +12092,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="439" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>255</v>
       </c>
@@ -12122,7 +12121,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="440" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>375</v>
       </c>
@@ -12202,7 +12201,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="444" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>230</v>
       </c>
@@ -12222,7 +12221,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="445" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>379</v>
       </c>
@@ -12242,7 +12241,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="446" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>233</v>
       </c>
@@ -12262,7 +12261,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="447" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>348</v>
       </c>
@@ -12282,7 +12281,7 @@
         <v>45207</v>
       </c>
     </row>
-    <row r="448" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>45</v>
       </c>
@@ -12308,7 +12307,7 @@
         <v>45206</v>
       </c>
     </row>
-    <row r="449" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>380</v>
       </c>
@@ -12328,7 +12327,7 @@
         <v>45206</v>
       </c>
     </row>
-    <row r="450" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>381</v>
       </c>
@@ -12348,7 +12347,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="451" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>382</v>
       </c>
@@ -12368,7 +12367,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="452" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>383</v>
       </c>
@@ -12388,7 +12387,7 @@
         <v>45204</v>
       </c>
     </row>
-    <row r="453" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>384</v>
       </c>
@@ -12468,7 +12467,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="457" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>387</v>
       </c>
@@ -12488,7 +12487,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="458" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>388</v>
       </c>
@@ -12508,7 +12507,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="459" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>389</v>
       </c>
@@ -12528,7 +12527,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="460" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>82</v>
       </c>
@@ -12548,7 +12547,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="461" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>344</v>
       </c>
@@ -12568,7 +12567,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="462" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>390</v>
       </c>
@@ -12588,7 +12587,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="463" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>23</v>
       </c>
@@ -12614,7 +12613,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="464" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>349</v>
       </c>
@@ -12643,7 +12642,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="465" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>391</v>
       </c>
@@ -12663,7 +12662,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="466" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>392</v>
       </c>
@@ -12683,7 +12682,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="467" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>393</v>
       </c>
@@ -12703,7 +12702,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="468" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>394</v>
       </c>
@@ -12723,7 +12722,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="469" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>395</v>
       </c>
@@ -12743,7 +12742,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="470" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>396</v>
       </c>
@@ -12763,7 +12762,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="471" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>232</v>
       </c>
@@ -12783,7 +12782,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="472" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>104</v>
       </c>
@@ -12823,7 +12822,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="474" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>398</v>
       </c>
@@ -12843,7 +12842,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="475" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>399</v>
       </c>
@@ -12863,7 +12862,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="476" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
         <v>400</v>
       </c>
@@ -12886,7 +12885,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="477" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>401</v>
       </c>
@@ -12906,7 +12905,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="478" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
         <v>402</v>
       </c>
@@ -12935,7 +12934,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="479" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
         <v>403</v>
       </c>
@@ -12955,7 +12954,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="480" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
         <v>404</v>
       </c>
@@ -12975,7 +12974,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="481" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>405</v>
       </c>
@@ -13004,7 +13003,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="482" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>406</v>
       </c>
@@ -13024,7 +13023,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="483" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>407</v>
       </c>
@@ -13064,7 +13063,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="485" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>409</v>
       </c>
@@ -13084,7 +13083,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="486" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>217</v>
       </c>
@@ -13104,7 +13103,7 @@
         <v>45198</v>
       </c>
     </row>
-    <row r="487" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>45</v>
       </c>
@@ -13130,7 +13129,7 @@
         <v>45195</v>
       </c>
     </row>
-    <row r="488" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>410</v>
       </c>
@@ -13150,7 +13149,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="489" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>411</v>
       </c>
@@ -13270,7 +13269,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="495" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>361</v>
       </c>
@@ -13290,7 +13289,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="496" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>417</v>
       </c>
@@ -13310,7 +13309,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="497" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
         <v>418</v>
       </c>
@@ -13330,7 +13329,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="498" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
         <v>419</v>
       </c>
@@ -13350,7 +13349,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="499" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>420</v>
       </c>
@@ -13370,7 +13369,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="500" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
         <v>230</v>
       </c>
@@ -13390,7 +13389,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="501" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>421</v>
       </c>
@@ -13410,7 +13409,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="502" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
         <v>422</v>
       </c>
@@ -13430,7 +13429,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="503" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
         <v>88</v>
       </c>
@@ -13450,7 +13449,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="504" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
         <v>423</v>
       </c>
@@ -13470,7 +13469,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="505" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
         <v>424</v>
       </c>
@@ -13490,7 +13489,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="506" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
         <v>425</v>
       </c>
@@ -13510,7 +13509,7 @@
         <v>45191</v>
       </c>
     </row>
-    <row r="507" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
         <v>426</v>
       </c>
@@ -13530,7 +13529,7 @@
         <v>45190</v>
       </c>
     </row>
-    <row r="508" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
         <v>427</v>
       </c>
@@ -13570,7 +13569,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="510" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
         <v>429</v>
       </c>
@@ -13610,7 +13609,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="512" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
         <v>431</v>
       </c>
@@ -13630,7 +13629,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="513" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>29</v>
       </c>
@@ -13656,7 +13655,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="514" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
         <v>23</v>
       </c>
@@ -13682,7 +13681,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="515" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>109</v>
       </c>
@@ -13702,7 +13701,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="516" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
         <v>432</v>
       </c>
@@ -13722,7 +13721,7 @@
         <v>45186</v>
       </c>
     </row>
-    <row r="517" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>433</v>
       </c>
@@ -13742,7 +13741,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="518" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
         <v>39</v>
       </c>
@@ -13768,7 +13767,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="519" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
         <v>434</v>
       </c>
@@ -13788,7 +13787,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="520" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
         <v>435</v>
       </c>
@@ -13808,7 +13807,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="521" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
         <v>436</v>
       </c>
@@ -13828,7 +13827,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="522" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
         <v>437</v>
       </c>
@@ -13848,7 +13847,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="523" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
         <v>63</v>
       </c>
@@ -13877,7 +13876,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="524" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
         <v>89</v>
       </c>
@@ -13897,7 +13896,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="525" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
         <v>250</v>
       </c>
@@ -13937,7 +13936,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="527" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
         <v>439</v>
       </c>
@@ -13957,7 +13956,7 @@
         <v>45183</v>
       </c>
     </row>
-    <row r="528" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
         <v>440</v>
       </c>
@@ -14146,7 +14145,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="537" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>110</v>
       </c>
@@ -14166,7 +14165,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="538" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>449</v>
       </c>
@@ -14186,7 +14185,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="539" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>395</v>
       </c>
@@ -14206,7 +14205,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="540" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>450</v>
       </c>
@@ -14226,7 +14225,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="541" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>451</v>
       </c>
@@ -14246,7 +14245,7 @@
         <v>45181</v>
       </c>
     </row>
-    <row r="542" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>103</v>
       </c>
@@ -14286,7 +14285,7 @@
         <v>45179</v>
       </c>
     </row>
-    <row r="544" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>453</v>
       </c>
@@ -14306,7 +14305,7 @@
         <v>45179</v>
       </c>
     </row>
-    <row r="545" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
         <v>454</v>
       </c>
@@ -14326,7 +14325,7 @@
         <v>45179</v>
       </c>
     </row>
-    <row r="546" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
         <v>455</v>
       </c>
@@ -14352,7 +14351,7 @@
         <v>45179</v>
       </c>
     </row>
-    <row r="547" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
         <v>456</v>
       </c>
@@ -14372,7 +14371,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="548" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
         <v>411</v>
       </c>
@@ -14392,7 +14391,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="549" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
         <v>457</v>
       </c>
@@ -14412,7 +14411,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="550" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
         <v>458</v>
       </c>
@@ -14432,7 +14431,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="551" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
         <v>435</v>
       </c>
@@ -14452,7 +14451,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="552" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
         <v>459</v>
       </c>
@@ -14512,7 +14511,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="555" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
         <v>182</v>
       </c>
@@ -14532,7 +14531,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="556" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
         <v>462</v>
       </c>
@@ -14632,7 +14631,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="561" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>465</v>
       </c>
@@ -14652,7 +14651,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="562" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>466</v>
       </c>
@@ -14672,7 +14671,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="563" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>232</v>
       </c>
@@ -14692,7 +14691,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="564" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
         <v>75</v>
       </c>
@@ -14718,7 +14717,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="565" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>231</v>
       </c>
@@ -14738,7 +14737,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="566" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
         <v>467</v>
       </c>
@@ -14758,7 +14757,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="567" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>250</v>
       </c>
@@ -14778,7 +14777,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="568" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
         <v>468</v>
       </c>
@@ -14798,7 +14797,7 @@
         <v>45176</v>
       </c>
     </row>
-    <row r="569" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>469</v>
       </c>
@@ -14838,7 +14837,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="571" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
         <v>346</v>
       </c>
@@ -14858,7 +14857,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="572" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
         <v>23</v>
       </c>
@@ -14884,7 +14883,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="573" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
         <v>471</v>
       </c>
@@ -14904,7 +14903,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="574" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
         <v>472</v>
       </c>
@@ -14924,7 +14923,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="575" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
         <v>473</v>
       </c>
@@ -14944,7 +14943,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="576" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
         <v>474</v>
       </c>
@@ -14973,7 +14972,7 @@
         <v>45174</v>
       </c>
     </row>
-    <row r="577" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
         <v>475</v>
       </c>
@@ -14993,7 +14992,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="578" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
         <v>476</v>
       </c>
@@ -15053,7 +15052,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="581" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
         <v>479</v>
       </c>
@@ -15073,7 +15072,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="582" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="582" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A582" t="s">
         <v>480</v>
       </c>
@@ -15093,7 +15092,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="583" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A583" t="s">
         <v>61</v>
       </c>
@@ -15113,7 +15112,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="584" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A584" t="s">
         <v>481</v>
       </c>
@@ -15133,7 +15132,7 @@
         <v>45171</v>
       </c>
     </row>
-    <row r="585" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
         <v>361</v>
       </c>
@@ -15173,7 +15172,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="587" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
         <v>230</v>
       </c>
@@ -15193,7 +15192,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="588" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
         <v>483</v>
       </c>
@@ -15239,7 +15238,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="590" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
         <v>116</v>
       </c>
@@ -15319,7 +15318,7 @@
         <v>45168</v>
       </c>
     </row>
-    <row r="594" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
         <v>487</v>
       </c>
@@ -15339,7 +15338,7 @@
         <v>45168</v>
       </c>
     </row>
-    <row r="595" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
         <v>488</v>
       </c>
@@ -15379,7 +15378,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="597" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
         <v>45</v>
       </c>
@@ -15405,7 +15404,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="598" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
         <v>91</v>
       </c>
@@ -15425,7 +15424,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="599" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
         <v>490</v>
       </c>
@@ -15445,7 +15444,7 @@
         <v>45166</v>
       </c>
     </row>
-    <row r="600" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
         <v>491</v>
       </c>
@@ -15465,7 +15464,7 @@
         <v>45166</v>
       </c>
     </row>
-    <row r="601" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
         <v>63</v>
       </c>
@@ -15494,7 +15493,7 @@
         <v>45166</v>
       </c>
     </row>
-    <row r="602" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
         <v>492</v>
       </c>
@@ -15514,7 +15513,7 @@
         <v>45166</v>
       </c>
     </row>
-    <row r="603" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
         <v>131</v>
       </c>
@@ -15534,7 +15533,7 @@
         <v>45165</v>
       </c>
     </row>
-    <row r="604" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
         <v>291</v>
       </c>
@@ -15654,7 +15653,7 @@
         <v>45164</v>
       </c>
     </row>
-    <row r="610" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
         <v>29</v>
       </c>
@@ -15680,7 +15679,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="611" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A611" t="s">
         <v>499</v>
       </c>
@@ -15700,7 +15699,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="612" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
         <v>500</v>
       </c>
@@ -15729,7 +15728,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="613" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
         <v>291</v>
       </c>
@@ -15749,7 +15748,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="614" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
         <v>502</v>
       </c>
@@ -15789,7 +15788,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="616" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
         <v>503</v>
       </c>
@@ -15809,7 +15808,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="617" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A617" t="s">
         <v>189</v>
       </c>
@@ -15829,7 +15828,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="618" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A618" t="s">
         <v>504</v>
       </c>
@@ -15849,7 +15848,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="619" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A619" t="s">
         <v>45</v>
       </c>
@@ -15875,7 +15874,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="620" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A620" t="s">
         <v>505</v>
       </c>
@@ -15895,7 +15894,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="621" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A621" t="s">
         <v>506</v>
       </c>
@@ -15915,7 +15914,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="622" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A622" t="s">
         <v>507</v>
       </c>
@@ -15935,7 +15934,7 @@
         <v>45161</v>
       </c>
     </row>
-    <row r="623" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="623" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A623" t="s">
         <v>508</v>
       </c>
@@ -15955,7 +15954,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="624" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
         <v>509</v>
       </c>
@@ -16015,7 +16014,7 @@
         <v>45155</v>
       </c>
     </row>
-    <row r="627" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="627" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A627" t="s">
         <v>512</v>
       </c>
@@ -16055,7 +16054,7 @@
         <v>45155</v>
       </c>
     </row>
-    <row r="629" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A629" t="s">
         <v>182</v>
       </c>
@@ -16075,7 +16074,7 @@
         <v>45155</v>
       </c>
     </row>
-    <row r="630" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A630" t="s">
         <v>514</v>
       </c>
@@ -16095,7 +16094,7 @@
         <v>45155</v>
       </c>
     </row>
-    <row r="631" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A631" t="s">
         <v>515</v>
       </c>
@@ -16115,7 +16114,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="632" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="632" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A632" t="s">
         <v>332</v>
       </c>
@@ -16135,7 +16134,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="633" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="633" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A633" t="s">
         <v>291</v>
       </c>
@@ -16175,7 +16174,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="635" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A635" t="s">
         <v>517</v>
       </c>
@@ -16195,7 +16194,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="636" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A636" t="s">
         <v>518</v>
       </c>
@@ -16215,7 +16214,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="637" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="637" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A637" t="s">
         <v>519</v>
       </c>
@@ -16235,7 +16234,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="638" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A638" t="s">
         <v>89</v>
       </c>
@@ -16255,7 +16254,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="639" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A639" t="s">
         <v>39</v>
       </c>
@@ -16281,7 +16280,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="640" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A640" t="s">
         <v>520</v>
       </c>
@@ -16301,7 +16300,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="641" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="641" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A641" t="s">
         <v>521</v>
       </c>
@@ -16321,7 +16320,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="642" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="642" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A642" t="s">
         <v>230</v>
       </c>
@@ -16341,7 +16340,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="643" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="643" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A643" t="s">
         <v>522</v>
       </c>
@@ -16367,7 +16366,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="644" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="644" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A644" t="s">
         <v>23</v>
       </c>
@@ -16393,7 +16392,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="645" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="645" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A645" t="s">
         <v>82</v>
       </c>
@@ -16453,7 +16452,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="648" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="648" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A648" t="s">
         <v>525</v>
       </c>
@@ -16473,7 +16472,7 @@
         <v>45153</v>
       </c>
     </row>
-    <row r="649" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="649" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A649" t="s">
         <v>526</v>
       </c>
@@ -16513,7 +16512,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="651" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="651" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A651" t="s">
         <v>170</v>
       </c>
@@ -16553,7 +16552,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="653" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="653" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A653" t="s">
         <v>530</v>
       </c>
@@ -16573,7 +16572,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="654" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="654" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A654" t="s">
         <v>531</v>
       </c>
@@ -16593,7 +16592,7 @@
         <v>45150</v>
       </c>
     </row>
-    <row r="655" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="655" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A655" t="s">
         <v>532</v>
       </c>
@@ -16613,7 +16612,7 @@
         <v>45150</v>
       </c>
     </row>
-    <row r="656" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="656" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A656" t="s">
         <v>63</v>
       </c>
@@ -16642,7 +16641,7 @@
         <v>45150</v>
       </c>
     </row>
-    <row r="657" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
         <v>348</v>
       </c>
@@ -16722,7 +16721,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="661" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
         <v>536</v>
       </c>
@@ -16742,7 +16741,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="662" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="662" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
         <v>537</v>
       </c>
@@ -16762,7 +16761,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="663" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="663" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
         <v>538</v>
       </c>
@@ -16802,7 +16801,7 @@
         <v>45140</v>
       </c>
     </row>
-    <row r="665" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
         <v>540</v>
       </c>
@@ -16822,7 +16821,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="666" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
         <v>32</v>
       </c>
@@ -16871,7 +16870,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="668" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="668" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A668" t="s">
         <v>82</v>
       </c>
@@ -16892,13 +16891,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L668" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Groceries"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L668" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -16909,7 +16902,7 @@
   <dimension ref="A1:L104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19988,7 +19981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14458C0-5F51-434B-B68D-A2BAF9BBF511}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>

</xml_diff>